<commit_message>
add lista de pedidos PDF
</commit_message>
<xml_diff>
--- a/pedidos/pedidos.xlsx
+++ b/pedidos/pedidos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="168">
   <si>
     <t>Numero_Pedido</t>
   </si>
@@ -487,10 +487,7 @@
     <t>11/06/2025 08:36</t>
   </si>
   <si>
-    <t>10/06/2025 13:10</t>
-  </si>
-  <si>
-    <t>09/06/2025 19:55</t>
+    <t>02/07/2025 14:28</t>
   </si>
   <si>
     <t>09/06/2025 19:59</t>
@@ -511,7 +508,16 @@
     <t>Sistema Automático</t>
   </si>
   <si>
+    <t>Sistema (PDF Exportado)</t>
+  </si>
+  <si>
     <t>09/06/2025 14:57</t>
+  </si>
+  <si>
+    <t>02/07/2025 14:12</t>
+  </si>
+  <si>
+    <t>02/07/2025 14:13</t>
   </si>
 </sst>
 </file>
@@ -982,10 +988,10 @@
         <v>151</v>
       </c>
       <c r="N2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R2" t="s">
         <v>151</v>
@@ -1032,16 +1038,16 @@
         <v>152</v>
       </c>
       <c r="N3" t="s">
+        <v>161</v>
+      </c>
+      <c r="O3" t="s">
         <v>162</v>
-      </c>
-      <c r="O3" t="s">
-        <v>163</v>
       </c>
       <c r="P3" t="s">
         <v>165</v>
       </c>
       <c r="Q3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R3" t="s">
         <v>152</v>
@@ -1088,16 +1094,16 @@
         <v>153</v>
       </c>
       <c r="N4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R4" t="s">
         <v>153</v>
       </c>
       <c r="S4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -1141,16 +1147,16 @@
         <v>154</v>
       </c>
       <c r="N5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R5" t="s">
         <v>154</v>
       </c>
       <c r="S5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -1194,10 +1200,10 @@
         <v>47</v>
       </c>
       <c r="N6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -1241,16 +1247,16 @@
         <v>155</v>
       </c>
       <c r="N7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R7" t="s">
         <v>155</v>
       </c>
       <c r="S7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -1294,16 +1300,16 @@
         <v>156</v>
       </c>
       <c r="N8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P8" t="s">
         <v>156</v>
       </c>
       <c r="S8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1338,19 +1344,31 @@
         <v>133</v>
       </c>
       <c r="K9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L9" t="s">
         <v>150</v>
       </c>
       <c r="M9" t="s">
-        <v>50</v>
+        <v>157</v>
       </c>
       <c r="N9" t="s">
         <v>164</v>
       </c>
+      <c r="O9" t="s">
+        <v>164</v>
+      </c>
+      <c r="P9" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>164</v>
+      </c>
+      <c r="R9" t="s">
+        <v>157</v>
+      </c>
       <c r="S9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1394,16 +1412,22 @@
         <v>157</v>
       </c>
       <c r="N10" t="s">
-        <v>163</v>
+        <v>164</v>
+      </c>
+      <c r="O10" t="s">
+        <v>164</v>
+      </c>
+      <c r="P10" t="s">
+        <v>167</v>
       </c>
       <c r="Q10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R10" t="s">
         <v>157</v>
       </c>
       <c r="S10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1444,19 +1468,25 @@
         <v>150</v>
       </c>
       <c r="M11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N11" t="s">
-        <v>163</v>
+        <v>164</v>
+      </c>
+      <c r="O11" t="s">
+        <v>164</v>
+      </c>
+      <c r="P11" t="s">
+        <v>167</v>
       </c>
       <c r="Q11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1497,19 +1527,19 @@
         <v>150</v>
       </c>
       <c r="M12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1553,10 +1583,10 @@
         <v>54</v>
       </c>
       <c r="N13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1600,10 +1630,10 @@
         <v>55</v>
       </c>
       <c r="N14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1647,10 +1677,10 @@
         <v>56</v>
       </c>
       <c r="N15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1694,10 +1724,10 @@
         <v>57</v>
       </c>
       <c r="N16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -1741,10 +1771,10 @@
         <v>58</v>
       </c>
       <c r="N17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -1785,19 +1815,19 @@
         <v>150</v>
       </c>
       <c r="M18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -1841,10 +1871,10 @@
         <v>60</v>
       </c>
       <c r="N19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -1882,10 +1912,10 @@
         <v>61</v>
       </c>
       <c r="N20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:19">
@@ -1923,10 +1953,10 @@
         <v>62</v>
       </c>
       <c r="N21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -1970,10 +2000,10 @@
         <v>63</v>
       </c>
       <c r="N22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -2017,10 +2047,10 @@
         <v>64</v>
       </c>
       <c r="N23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:19">
@@ -2058,10 +2088,10 @@
         <v>65</v>
       </c>
       <c r="N24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -2105,10 +2135,10 @@
         <v>66</v>
       </c>
       <c r="N25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -2149,19 +2179,19 @@
         <v>150</v>
       </c>
       <c r="M26" t="s">
+        <v>160</v>
+      </c>
+      <c r="N26" t="s">
         <v>161</v>
       </c>
-      <c r="N26" t="s">
-        <v>162</v>
-      </c>
       <c r="Q26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>